<commit_message>
Forgot to save K10 scoring calculator?
</commit_message>
<xml_diff>
--- a/data processing/K10/K10 scoring calculator.xlsx
+++ b/data processing/K10/K10 scoring calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephan Taljaard\Documents\Dam-simulation\data processing\K3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephan Taljaard\Documents\Dam-simulation\data processing\K10\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -856,46 +856,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>3800</c:v>
+                  <c:v>13360.52267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3800</c:v>
+                  <c:v>13198.17489</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3800</c:v>
+                  <c:v>11593.883669999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3800</c:v>
+                  <c:v>12077.97522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3800</c:v>
+                  <c:v>13375.281559999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3800</c:v>
+                  <c:v>13115.52511</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3800</c:v>
+                  <c:v>12126.67956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3800</c:v>
+                  <c:v>12714.083329999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>899.33333333333303</c:v>
+                  <c:v>11841.343999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -910,58 +910,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>392.666666666666</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1900</c:v>
+                  <c:v>670.05355559999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3800</c:v>
+                  <c:v>12875.056</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3800</c:v>
+                  <c:v>10557.685219999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3800</c:v>
+                  <c:v>11050.62667</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3800</c:v>
+                  <c:v>13351.66733</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3800</c:v>
+                  <c:v>13147.99467</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3800</c:v>
+                  <c:v>12753.93233</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3800</c:v>
+                  <c:v>12786.401889999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3800</c:v>
+                  <c:v>13748.68144</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3800</c:v>
+                  <c:v>8640.6579999999994</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3800</c:v>
+                  <c:v>1908.324333</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -973,31 +973,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.1111111111111</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3800</c:v>
+                  <c:v>11875.77844</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3800</c:v>
+                  <c:v>13339.86022</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3800</c:v>
+                  <c:v>12777.546560000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3800</c:v>
+                  <c:v>11356.26556</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1042,46 +1042,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>3800</c:v>
+                  <c:v>13360.52267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3800</c:v>
+                  <c:v>13198.17489</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3800</c:v>
+                  <c:v>11593.883669999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3800</c:v>
+                  <c:v>12077.97522</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3800</c:v>
+                  <c:v>13375.281559999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3800</c:v>
+                  <c:v>13115.52511</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3800</c:v>
+                  <c:v>12126.67956</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3800</c:v>
+                  <c:v>12714.083329999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>899.33333330000005</c:v>
+                  <c:v>11841.343999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -1096,58 +1096,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>392.66666670000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1900</c:v>
+                  <c:v>670.05355559999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3800</c:v>
+                  <c:v>12875.056</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3800</c:v>
+                  <c:v>10557.685219999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3800</c:v>
+                  <c:v>11050.62667</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3800</c:v>
+                  <c:v>13351.66733</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3800</c:v>
+                  <c:v>13147.99467</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3800</c:v>
+                  <c:v>12753.93233</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3800</c:v>
+                  <c:v>12786.401889999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3800</c:v>
+                  <c:v>13748.68144</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3800</c:v>
+                  <c:v>8640.6579999999994</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3800</c:v>
+                  <c:v>1908.324333</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>0</c:v>
@@ -1159,31 +1159,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>97.111111109999996</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3800</c:v>
+                  <c:v>11875.77844</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3800</c:v>
+                  <c:v>13339.86022</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3800</c:v>
+                  <c:v>12777.546560000001</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3800</c:v>
+                  <c:v>11356.26556</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1228,49 +1228,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
                 <c:pt idx="0">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3800</c:v>
+                  <c:v>13032.875330000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3800</c:v>
+                  <c:v>11893.48911</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3800</c:v>
+                  <c:v>13772.29567</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3800</c:v>
+                  <c:v>11608.64256</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3800</c:v>
+                  <c:v>10781.62667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.0555555560000001</c:v>
+                  <c:v>4.4276666669999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -1285,58 +1285,58 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>442.27777780000002</c:v>
+                  <c:v>875.20211110000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3800</c:v>
+                  <c:v>13817.89878</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3800</c:v>
+                  <c:v>12668.63867</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3800</c:v>
+                  <c:v>10895.4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3800</c:v>
+                  <c:v>9709.6564440000002</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3800</c:v>
+                  <c:v>12659.47544</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3800</c:v>
+                  <c:v>12184.239219999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3800</c:v>
+                  <c:v>13211.45789</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3800</c:v>
+                  <c:v>12135.529329999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3800</c:v>
+                  <c:v>4809.9218890000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0555555560000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0</c:v>
@@ -1348,28 +1348,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3798.9444440000002</c:v>
+                  <c:v>12368.57589</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3800</c:v>
+                  <c:v>13821</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3800</c:v>
+                  <c:v>13392.99222</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3800</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3336.6111110000002</c:v>
+                  <c:v>11164.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="H1" s="17">
         <f>SUMPRODUCT(F3:F6,G3:G6)</f>
-        <v>3800</v>
+        <v>16746.599999999999</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
@@ -2470,31 +2470,31 @@
       </c>
       <c r="M2" s="1">
         <f>COUNTIF($A$2:$A$49,K2)*$H$1</f>
-        <v>60800</v>
+        <v>267945.59999999998</v>
       </c>
       <c r="Q2">
-        <v>3800</v>
+        <v>13360.52267</v>
       </c>
       <c r="R2">
-        <v>3800</v>
+        <v>13360.52267</v>
       </c>
       <c r="S2">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="U2" t="s">
         <v>10</v>
       </c>
       <c r="V2">
         <f>SUM(Q2:Q49)/2</f>
-        <v>71944.555555555562</v>
+        <v>235466.30111429997</v>
       </c>
       <c r="W2">
         <f>SUM(R2:R49)/2</f>
-        <v>71944.555555555009</v>
+        <v>235466.30111429997</v>
       </c>
       <c r="X2">
         <f>SUM(S2:S49)/2</f>
-        <v>72189.972221956006</v>
+        <v>233659.17244538353</v>
       </c>
       <c r="AC2" t="s">
         <v>7</v>
@@ -2513,12 +2513,14 @@
       <c r="B3">
         <v>0.39020000000000005</v>
       </c>
-      <c r="E3" s="10"/>
+      <c r="E3" s="10">
+        <v>27</v>
+      </c>
       <c r="F3">
-        <v>1900</v>
+        <v>2925.6</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -2528,16 +2530,16 @@
       </c>
       <c r="M3" s="1">
         <f t="shared" ref="M3:M4" si="0">COUNTIF($A$2:$A$49,K3)*$H$1</f>
-        <v>83600</v>
+        <v>368425.19999999995</v>
       </c>
       <c r="Q3">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="R3">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="S3">
-        <v>3800</v>
+        <v>13032.875330000001</v>
       </c>
       <c r="AC3">
         <v>1</v>
@@ -2556,6 +2558,15 @@
       <c r="B4">
         <v>0.39020000000000005</v>
       </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>2656.6</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
       <c r="K4">
         <v>3</v>
       </c>
@@ -2564,16 +2575,16 @@
       </c>
       <c r="M4" s="1">
         <f t="shared" si="0"/>
-        <v>38000</v>
+        <v>167466</v>
       </c>
       <c r="Q4">
-        <v>3800</v>
+        <v>13198.17489</v>
       </c>
       <c r="R4">
-        <v>3800</v>
+        <v>13198.17489</v>
       </c>
       <c r="S4">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -2584,13 +2595,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q5">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R5">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S5">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="U5" t="s">
         <v>11</v>
@@ -2604,28 +2615,28 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q6">
-        <v>3800</v>
+        <v>11593.883669999999</v>
       </c>
       <c r="R6">
-        <v>3800</v>
+        <v>11593.883669999999</v>
       </c>
       <c r="S6">
-        <v>3800</v>
+        <v>11893.48911</v>
       </c>
       <c r="U6">
         <v>1</v>
       </c>
       <c r="V6" s="1">
         <f>IF(V2&lt;M2,V2,M2)</f>
-        <v>60800</v>
+        <v>235466.30111429997</v>
       </c>
       <c r="W6" s="1">
         <f>IF(W2&lt;M2,W2,M2)</f>
-        <v>60800</v>
+        <v>235466.30111429997</v>
       </c>
       <c r="X6" s="1">
         <f>IF(X2&lt;M2,X2,M2)</f>
-        <v>60800</v>
+        <v>233659.17244538353</v>
       </c>
       <c r="AB6" t="s">
         <v>17</v>
@@ -2642,28 +2653,28 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q7">
-        <v>3800</v>
+        <v>12077.97522</v>
       </c>
       <c r="R7">
-        <v>3800</v>
+        <v>12077.97522</v>
       </c>
       <c r="S7">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="U7">
         <v>2</v>
       </c>
       <c r="V7" s="1">
         <f>IF((V2-V6)&gt;$M$3,$M$3,V2-V6)</f>
-        <v>11144.555555555562</v>
+        <v>0</v>
       </c>
       <c r="W7" s="1">
         <f t="shared" ref="W7:X7" si="1">IF((W2-W6)&gt;$M$3,$M$3,W2-W6)</f>
-        <v>11144.555555555009</v>
+        <v>0</v>
       </c>
       <c r="X7" s="1">
         <f t="shared" si="1"/>
-        <v>11389.972221956006</v>
+        <v>0</v>
       </c>
       <c r="AC7" t="s">
         <v>7</v>
@@ -2683,13 +2694,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q8">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R8">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S8">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="U8">
         <v>3</v>
@@ -2707,10 +2718,10 @@
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE8">
         <v>1</v>
@@ -2724,25 +2735,25 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q9">
-        <v>3800</v>
+        <v>13375.281559999999</v>
       </c>
       <c r="R9">
-        <v>3800</v>
+        <v>13375.281559999999</v>
       </c>
       <c r="S9">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="V9" s="3">
         <f>V6*$B$2+V7*$B$14+V8*$B$16</f>
-        <v>30579.17612222223</v>
+        <v>91878.95069479986</v>
       </c>
       <c r="W9" s="3">
         <f t="shared" ref="W9" si="3">W6*$B$2+W7*$B$14+W8*$B$16</f>
-        <v>30579.176122221888</v>
+        <v>91878.95069479986</v>
       </c>
       <c r="X9" s="3">
         <f>X6*$B$2+X7*$B$14+X8*$B$16</f>
-        <v>30730.131913725141</v>
+        <v>91173.80908818866</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -2753,13 +2764,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q10">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="R10">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="S10">
-        <v>3800</v>
+        <v>13772.29567</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -2770,13 +2781,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q11">
-        <v>3800</v>
+        <v>13115.52511</v>
       </c>
       <c r="R11">
-        <v>3800</v>
+        <v>13115.52511</v>
       </c>
       <c r="S11">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="U11" t="s">
         <v>12</v>
@@ -2790,28 +2801,28 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q12">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R12">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S12">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="U12">
         <v>1</v>
       </c>
       <c r="V12" s="1">
         <f>SUMIF($A$2:$A$49,$U12,Q$2:Q$49)/2</f>
-        <v>30400</v>
+        <v>102207.82739999998</v>
       </c>
       <c r="W12" s="1">
         <f t="shared" ref="W12:X12" si="4">SUMIF($A$2:$A$49,$U12,R$2:R$49)/2</f>
-        <v>30400</v>
+        <v>102207.82739999998</v>
       </c>
       <c r="X12" s="1">
         <f t="shared" si="4"/>
-        <v>30168.305555499999</v>
+        <v>99895.847444999992</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -2822,28 +2833,28 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q13">
-        <v>3800</v>
+        <v>12126.67956</v>
       </c>
       <c r="R13">
-        <v>3800</v>
+        <v>12126.67956</v>
       </c>
       <c r="S13">
-        <v>3800</v>
+        <v>11608.64256</v>
       </c>
       <c r="U13">
         <v>2</v>
       </c>
       <c r="V13" s="1">
         <f t="shared" ref="V13:V14" si="5">SUMIF($A$2:$A$49,$U13,Q$2:Q$49)/2</f>
-        <v>40349.666666666664</v>
+        <v>132923.4469365</v>
       </c>
       <c r="W13" s="1">
         <f t="shared" ref="W13:W14" si="6">SUMIF($A$2:$A$49,$U13,R$2:R$49)/2</f>
-        <v>40349.666666650002</v>
+        <v>132923.4469365</v>
       </c>
       <c r="X13" s="1">
         <f t="shared" ref="X13:X14" si="7">SUMIF($A$2:$A$49,$U13,S$2:S$49)/2</f>
-        <v>41799.472221999997</v>
+        <v>133323.51011149999</v>
       </c>
       <c r="AB13" s="5" t="s">
         <v>20</v>
@@ -2857,28 +2868,28 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q14">
-        <v>3800</v>
+        <v>12714.083329999999</v>
       </c>
       <c r="R14">
-        <v>3800</v>
+        <v>12714.083329999999</v>
       </c>
       <c r="S14">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="U14">
         <v>3</v>
       </c>
       <c r="V14" s="2">
         <f t="shared" si="5"/>
-        <v>1194.8888888888887</v>
+        <v>335.02677779999999</v>
       </c>
       <c r="W14" s="2">
         <f t="shared" si="6"/>
-        <v>1194.8888889049999</v>
+        <v>335.02677779999999</v>
       </c>
       <c r="X14" s="2">
         <f t="shared" si="7"/>
-        <v>222.19444445600001</v>
+        <v>439.81488888350003</v>
       </c>
       <c r="AB14" t="s">
         <v>21</v>
@@ -2895,25 +2906,25 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q15">
-        <v>899.33333333333303</v>
+        <v>11841.343999999999</v>
       </c>
       <c r="R15">
-        <v>899.33333330000005</v>
+        <v>11841.343999999999</v>
       </c>
       <c r="S15">
-        <v>3800</v>
+        <v>10781.62667</v>
       </c>
       <c r="V15" s="3">
         <f>V12*$B$2+V13*$B$14+V14*$B$16</f>
-        <v>37748.912677777778</v>
+        <v>121942.08639076322</v>
       </c>
       <c r="W15" s="3">
         <f t="shared" ref="W15" si="8">W12*$B$2+W13*$B$14+W14*$B$16</f>
-        <v>37748.912677781926</v>
+        <v>121942.08639076322</v>
       </c>
       <c r="X15" s="3">
         <f>X12*$B$2+X13*$B$14+X14*$B$16</f>
-        <v>37681.081147074183</v>
+        <v>121379.66932732893</v>
       </c>
       <c r="AB15" t="s">
         <v>22</v>
@@ -2936,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>1.0555555560000001</v>
+        <v>4.4276666669999996</v>
       </c>
       <c r="AB16" t="s">
         <v>23</v>
@@ -3000,15 +3011,15 @@
       </c>
       <c r="V19">
         <f>V9/V15</f>
-        <v>0.81006773316211922</v>
+        <v>0.75346382380545718</v>
       </c>
       <c r="W19">
         <f t="shared" ref="W19:X19" si="9">W9/W15</f>
-        <v>0.81006773316202119</v>
+        <v>0.75346382380545718</v>
       </c>
       <c r="X19">
         <f t="shared" si="9"/>
-        <v>0.81553211792892621</v>
+        <v>0.75114563743222074</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -3019,10 +3030,10 @@
         <v>0.89359999999999995</v>
       </c>
       <c r="Q20">
-        <v>392.666666666666</v>
+        <v>0</v>
       </c>
       <c r="R20">
-        <v>392.66666670000001</v>
+        <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
@@ -3039,13 +3050,13 @@
         <v>0.89359999999999995</v>
       </c>
       <c r="Q21">
-        <v>1900</v>
+        <v>670.05355559999998</v>
       </c>
       <c r="R21">
-        <v>1900</v>
+        <v>670.05355559999998</v>
       </c>
       <c r="S21">
-        <v>442.27777780000002</v>
+        <v>875.20211110000002</v>
       </c>
       <c r="AC21" t="s">
         <v>7</v>
@@ -3065,28 +3076,28 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q22">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R22">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S22">
-        <v>3800</v>
+        <v>13817.89878</v>
       </c>
       <c r="AB22" s="5" t="s">
         <v>13</v>
       </c>
       <c r="AC22">
         <f>(V19*$AC$14+AC3*$AC$15+AC8*$AC$16)/SUM($AC$14:$AC$16)</f>
-        <v>0.96201354663242389</v>
+        <v>0.55069276476109141</v>
       </c>
       <c r="AD22">
         <f>(W19*$AC$14+AD3*$AC$15+AD8*$AC$16)/SUM($AC$14:$AC$16)</f>
-        <v>0.96201354663240424</v>
+        <v>0.55069276476109141</v>
       </c>
       <c r="AE22">
         <f>(X19*$AC$14+AE3*$AC$15+AE8*$AC$16)/SUM($AC$14:$AC$16)</f>
-        <v>0.96310642358578524</v>
+        <v>0.95022912748644417</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -3097,13 +3108,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q23">
-        <v>3800</v>
+        <v>12875.056</v>
       </c>
       <c r="R23">
-        <v>3800</v>
+        <v>12875.056</v>
       </c>
       <c r="S23">
-        <v>3800</v>
+        <v>12668.63867</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -3114,13 +3125,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q24">
-        <v>3800</v>
+        <v>10557.685219999999</v>
       </c>
       <c r="R24">
-        <v>3800</v>
+        <v>10557.685219999999</v>
       </c>
       <c r="S24">
-        <v>3800</v>
+        <v>10895.4</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -3131,13 +3142,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q25">
-        <v>3800</v>
+        <v>11050.62667</v>
       </c>
       <c r="R25">
-        <v>3800</v>
+        <v>11050.62667</v>
       </c>
       <c r="S25">
-        <v>3800</v>
+        <v>9709.6564440000002</v>
       </c>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.25">
@@ -3148,13 +3159,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q26">
-        <v>3800</v>
+        <v>13351.66733</v>
       </c>
       <c r="R26">
-        <v>3800</v>
+        <v>13351.66733</v>
       </c>
       <c r="S26">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.25">
@@ -3165,13 +3176,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q27">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R27">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S27">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.25">
@@ -3182,13 +3193,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q28">
-        <v>3800</v>
+        <v>13147.99467</v>
       </c>
       <c r="R28">
-        <v>3800</v>
+        <v>13147.99467</v>
       </c>
       <c r="S28">
-        <v>3800</v>
+        <v>12659.47544</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.25">
@@ -3199,13 +3210,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q29">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="R29">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="S29">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -3216,13 +3227,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q30">
-        <v>3800</v>
+        <v>12753.93233</v>
       </c>
       <c r="R30">
-        <v>3800</v>
+        <v>12753.93233</v>
       </c>
       <c r="S30">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.25">
@@ -3233,13 +3244,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q31">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R31">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S31">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.25">
@@ -3250,13 +3261,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q32">
-        <v>3800</v>
+        <v>12786.401889999999</v>
       </c>
       <c r="R32">
-        <v>3800</v>
+        <v>12786.401889999999</v>
       </c>
       <c r="S32">
-        <v>3800</v>
+        <v>12184.239219999999</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -3267,13 +3278,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q33">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="R33">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
       <c r="S33">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -3284,13 +3295,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q34">
-        <v>3800</v>
+        <v>13748.68144</v>
       </c>
       <c r="R34">
-        <v>3800</v>
+        <v>13748.68144</v>
       </c>
       <c r="S34">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -3301,13 +3312,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q35">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R35">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S35">
-        <v>3800</v>
+        <v>13211.45789</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -3318,13 +3329,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q36">
-        <v>3800</v>
+        <v>8640.6579999999994</v>
       </c>
       <c r="R36">
-        <v>3800</v>
+        <v>8640.6579999999994</v>
       </c>
       <c r="S36">
-        <v>3800</v>
+        <v>12135.529329999999</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -3335,13 +3346,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q37">
-        <v>3800</v>
+        <v>1908.324333</v>
       </c>
       <c r="R37">
-        <v>3800</v>
+        <v>1908.324333</v>
       </c>
       <c r="S37">
-        <v>3800</v>
+        <v>4809.9218890000002</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -3358,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>1.0555555560000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -3403,10 +3414,10 @@
         <v>0.89359999999999995</v>
       </c>
       <c r="Q41">
-        <v>97.1111111111111</v>
+        <v>0</v>
       </c>
       <c r="R41">
-        <v>97.111111109999996</v>
+        <v>0</v>
       </c>
       <c r="S41">
         <v>0</v>
@@ -3420,13 +3431,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q42">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R42">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S42">
-        <v>3798.9444440000002</v>
+        <v>12368.57589</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3437,13 +3448,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q43">
-        <v>3800</v>
+        <v>11875.77844</v>
       </c>
       <c r="R43">
-        <v>3800</v>
+        <v>11875.77844</v>
       </c>
       <c r="S43">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -3454,13 +3465,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q44">
-        <v>3800</v>
+        <v>13339.86022</v>
       </c>
       <c r="R44">
-        <v>3800</v>
+        <v>13339.86022</v>
       </c>
       <c r="S44">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3471,13 +3482,13 @@
         <v>0.61509999999999998</v>
       </c>
       <c r="Q45">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R45">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S45">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3488,13 +3499,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q46">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R46">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S46">
-        <v>3800</v>
+        <v>13821</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3505,13 +3516,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q47">
-        <v>3800</v>
+        <v>12777.546560000001</v>
       </c>
       <c r="R47">
-        <v>3800</v>
+        <v>12777.546560000001</v>
       </c>
       <c r="S47">
-        <v>3800</v>
+        <v>13392.99222</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3522,13 +3533,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q48">
-        <v>3800</v>
+        <v>11356.26556</v>
       </c>
       <c r="R48">
-        <v>3800</v>
+        <v>11356.26556</v>
       </c>
       <c r="S48">
-        <v>3800</v>
+        <v>11164.4</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
@@ -3539,13 +3550,13 @@
         <v>0.39020000000000005</v>
       </c>
       <c r="Q49">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="R49">
-        <v>3800</v>
+        <v>13821</v>
       </c>
       <c r="S49">
-        <v>3336.6111110000002</v>
+        <v>11164.4</v>
       </c>
     </row>
   </sheetData>
@@ -3813,15 +3824,15 @@
       </c>
       <c r="D2">
         <f>'Simulation score'!AC22</f>
-        <v>0.96201354663242389</v>
+        <v>0.55069276476109141</v>
       </c>
       <c r="E2">
         <f>'Simulation score'!AD22</f>
-        <v>0.96201354663240424</v>
+        <v>0.55069276476109141</v>
       </c>
       <c r="F2">
         <f>'Simulation score'!AE22</f>
-        <v>0.96310642358578524</v>
+        <v>0.95022912748644417</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3851,15 +3862,15 @@
       <c r="C4" s="18"/>
       <c r="D4" s="18">
         <f>($C$2*D2+$C$3*D3)/SUM($C$2:$C$3)</f>
-        <v>0.75245347553272701</v>
+        <v>0.4782396209518387</v>
       </c>
       <c r="E4" s="18">
         <f>($C$2*E2+$C$3*E3)/SUM($C$2:$C$3)</f>
-        <v>0.82652754960678809</v>
+        <v>0.55231369502591277</v>
       </c>
       <c r="F4" s="18">
         <f>($C$2*F2+$C$3*F3)/SUM($C$2:$C$3)</f>
-        <v>0.97540428239052346</v>
+        <v>0.96681941832429608</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3871,15 +3882,15 @@
       </c>
       <c r="D5">
         <f t="shared" ref="D5:F6" si="0">$C2/SUM($C$2:$C$3)*D2*100</f>
-        <v>64.13423644216158</v>
+        <v>36.712850984072759</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>64.134236442160272</v>
+        <v>36.712850984072759</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>64.207094905719003</v>
+        <v>63.348608499096272</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3907,15 +3918,15 @@
       <c r="C7" s="15"/>
       <c r="D7" s="16">
         <f>D4*100</f>
-        <v>75.245347553272694</v>
+        <v>47.823962095183873</v>
       </c>
       <c r="E7" s="16">
         <f>E4*100</f>
-        <v>82.652754960678806</v>
+        <v>55.231369502591278</v>
       </c>
       <c r="F7" s="16">
         <f>F4*100</f>
-        <v>97.540428239052346</v>
+        <v>96.681941832429601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename "Simulation score" to "Performance score"
</commit_message>
<xml_diff>
--- a/data processing/K10/K10 scoring calculator.xlsx
+++ b/data processing/K10/K10 scoring calculator.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="Simulation score" sheetId="1" r:id="rId1"/>
+    <sheet name="Performance score" sheetId="1" r:id="rId1"/>
     <sheet name="Feature score" sheetId="2" r:id="rId2"/>
     <sheet name="Total score" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -85,9 +85,6 @@
     <t>1 = no cycling, 0 = cycling</t>
   </si>
   <si>
-    <t>Total simulation scores</t>
-  </si>
-  <si>
     <t>Weights</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>3-factor</t>
   </si>
   <si>
-    <t>Simulation score</t>
-  </si>
-  <si>
     <t>Feature score</t>
   </si>
   <si>
@@ -146,6 +140,12 @@
   </si>
   <si>
     <t>Monitoring and reporting</t>
+  </si>
+  <si>
+    <t>Total performancen scores</t>
+  </si>
+  <si>
+    <t>Performance score</t>
   </si>
 </sst>
 </file>
@@ -828,7 +828,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simulation score'!$Q$1</c:f>
+              <c:f>'Performance score'!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -851,7 +851,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Simulation score'!$Q$2:$Q$49</c:f>
+              <c:f>'Performance score'!$Q$2:$Q$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -1014,7 +1014,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simulation score'!$R$1</c:f>
+              <c:f>'Performance score'!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1037,7 +1037,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Simulation score'!$R$2:$R$49</c:f>
+              <c:f>'Performance score'!$R$2:$R$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -1200,7 +1200,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Simulation score'!$S$1</c:f>
+              <c:f>'Performance score'!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1223,7 +1223,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Simulation score'!$S$2:$S$49</c:f>
+              <c:f>'Performance score'!$S$2:$S$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="48"/>
@@ -2428,7 +2428,7 @@
         <v>3</v>
       </c>
       <c r="P1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="Q1" t="s">
         <v>7</v>
@@ -2857,7 +2857,7 @@
         <v>133323.51011149999</v>
       </c>
       <c r="AB13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -2892,7 +2892,7 @@
         <v>439.81488888350003</v>
       </c>
       <c r="AB14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AC14">
         <v>1</v>
@@ -2927,7 +2927,7 @@
         <v>121379.66932732893</v>
       </c>
       <c r="AB15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC15">
         <v>2</v>
@@ -2950,7 +2950,7 @@
         <v>4.4276666669999996</v>
       </c>
       <c r="AB16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AC16">
         <v>2</v>
@@ -3039,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="AB20" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -3636,7 +3636,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -3650,12 +3650,12 @@
         <v>8</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="12">
         <v>0</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="12">
         <v>2</v>
@@ -3683,7 +3683,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="12">
         <v>2</v>
@@ -3697,7 +3697,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="12">
         <v>1</v>
@@ -3711,7 +3711,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12">
         <v>1</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="12">
         <v>3</v>
@@ -3755,7 +3755,7 @@
     <row r="10" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="11">
         <f>COUNTA(A3:A8)*3</f>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="14">
         <f>B9/$B$11</f>
@@ -3796,14 +3796,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="4"/>
       <c r="C1" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>7</v>
@@ -3817,27 +3817,27 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>6</v>
       </c>
       <c r="D2">
-        <f>'Simulation score'!AC22</f>
+        <f>'Performance score'!AC22</f>
         <v>0.55069276476109141</v>
       </c>
       <c r="E2">
-        <f>'Simulation score'!AD22</f>
+        <f>'Performance score'!AD22</f>
         <v>0.55069276476109141</v>
       </c>
       <c r="F2">
-        <f>'Simulation score'!AE22</f>
+        <f>'Performance score'!AE22</f>
         <v>0.95022912748644417</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4">
         <v>3</v>
@@ -3857,7 +3857,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18">
@@ -3875,10 +3875,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:F6" si="0">$C2/SUM($C$2:$C$3)*D2*100</f>
@@ -3895,7 +3895,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4">
@@ -3913,7 +3913,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="15"/>
       <c r="D7" s="16">

</xml_diff>